<commit_message>
updated distribution parser in progress, #774
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-distribution.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-distribution.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Year</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Tank</t>
   </si>
   <si>
-    <t>Temp</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -74,7 +71,31 @@
     <t>Len (cm)</t>
   </si>
   <si>
-    <t>Collection</t>
+    <t>Year Collection</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Trough</t>
+  </si>
+  <si>
+    <t>Release Method</t>
+  </si>
+  <si>
+    <t>Truck Temp</t>
+  </si>
+  <si>
+    <t>River Temp</t>
+  </si>
+  <si>
+    <t>Acclimation Time (mins)</t>
+  </si>
+  <si>
+    <t>Lifestage</t>
+  </si>
+  <si>
+    <t>Weight (Kg)</t>
   </si>
 </sst>
 </file>
@@ -408,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:Q3"/>
+  <dimension ref="A3:X3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +442,7 @@
     <col min="17" max="17" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -435,43 +456,64 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="1" t="s">
+      <c r="V3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="X3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add individual distribution parser, #774
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-distribution.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-distribution.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Groups" sheetId="1" r:id="rId1"/>
+    <sheet name="Individuals" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Year</t>
   </si>
@@ -96,6 +97,18 @@
   </si>
   <si>
     <t>Weight (Kg)</t>
+  </si>
+  <si>
+    <t>PIT Tag</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Tissue (Y/N)</t>
+  </si>
+  <si>
+    <t>Vial</t>
   </si>
 </sst>
 </file>
@@ -431,15 +444,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -511,6 +530,108 @@
       </c>
       <c r="W3" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:X3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T7" sqref="T7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="X3" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
work on stock code report, add group container history method
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/mactaquac-distribution.xlsx
+++ b/bio_diversity/static/data_templates/mactaquac-distribution.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Groups" sheetId="1" r:id="rId1"/>
@@ -201,11 +201,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Enter trough names here if distributing from troughs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Optional</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q3" authorId="0" shapeId="0">
+    <comment ref="R3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -218,7 +231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R3" authorId="0" shapeId="0">
+    <comment ref="S3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -231,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S3" authorId="0" shapeId="0">
+    <comment ref="T3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -244,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T3" authorId="0" shapeId="0">
+    <comment ref="U3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -258,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U3" authorId="0" shapeId="0">
+    <comment ref="V3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -271,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V3" authorId="0" shapeId="0">
+    <comment ref="W3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -284,7 +297,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X3" authorId="0" shapeId="0">
+    <comment ref="Y3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -534,7 +547,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
@@ -964,26 +977,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:X3"/>
+  <dimension ref="A3:Y3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="8" max="8" width="28.28515625" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
-    <col min="14" max="15" width="25.140625" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" customWidth="1"/>
-    <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="25.140625" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1030,30 +1043,33 @@
         <v>29</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1068,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:X4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+    <sheetView topLeftCell="S1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>

</xml_diff>